<commit_message>
嗯嗯 Signed-off-by: disnio <291166364@qq.com>
</commit_message>
<xml_diff>
--- a/note/笔记本.xlsx
+++ b/note/笔记本.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="193">
   <si>
     <t>品牌</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -192,10 +192,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>68% ips 雾面 316尼特</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>69% ips 雾面</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -423,10 +419,6 @@
   </si>
   <si>
     <t>光影精灵5 Plus</t>
-  </si>
-  <si>
-    <t>USB2个，1个typeC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>4铜 2出风 2风扇</t>
@@ -767,10 +759,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>ZX7-CP5H2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>HM370，是GK5CM64(Z2Air)的神舟贴牌产品，属于Z7-KP7(G)Z的继承者。有高色域。典型的水桶机</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -828,6 +816,41 @@
   </si>
   <si>
     <t>！</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2+2.6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>150w（19V 7.89A）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>72% ips 雾面 316尼特</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>双烤模式下的，CPU与显卡双双到达了80度，CPU更是有82度的高温，但是CPU的频率并不高，只有默频的2.2Ghz，显卡的表现比较正常并没有出现降频的情况。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB2个，1个typeC</t>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://mp.weixin.qq.com/s?src=11&amp;timestamp=1565172616&amp;ver=1776&amp;signature=bO49aE6HMP6NLNOf9MuX31l15pJGexyu*FPg5T3fE5Pp0Lu4k3vzBuTsMyoSKLxEuzD8w9-kXG6Rer0bPKKFRtzEugLgPYP6UlF3U7jL3EMpg0Anp4lz3MIa3DxzNiZG&amp;new=1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZX7-CP5H2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>230w</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1016,7 +1039,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1050,7 +1073,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1187,6 +1210,9 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -1196,8 +1222,8 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1515,12 +1541,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T120"/>
+  <dimension ref="A1:T121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1538,7 +1564,7 @@
     <col min="11" max="11" width="10.75" customWidth="1"/>
     <col min="12" max="13" width="19.25" customWidth="1"/>
     <col min="14" max="14" width="7.125" customWidth="1"/>
-    <col min="15" max="15" width="10.875" customWidth="1"/>
+    <col min="15" max="15" width="16" customWidth="1"/>
     <col min="16" max="16" width="5.25" customWidth="1"/>
     <col min="17" max="17" width="8" style="1" customWidth="1"/>
     <col min="18" max="18" width="31.375" style="16" customWidth="1"/>
@@ -1584,7 +1610,7 @@
         <v>30</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>26</v>
@@ -1596,13 +1622,13 @@
         <v>5</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R1" s="41" t="s">
         <v>28</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="T1" s="17" t="s">
         <v>15</v>
@@ -1631,7 +1657,7 @@
         <v>21</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>40</v>
@@ -1657,13 +1683,13 @@
     </row>
     <row r="3" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2">
         <v>6099</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="2">
         <v>8</v>
@@ -1672,16 +1698,16 @@
         <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>33</v>
@@ -1695,13 +1721,13 @@
     </row>
     <row r="4" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C4" s="2">
         <v>4599</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="2">
         <v>8</v>
@@ -1710,10 +1736,10 @@
         <v>13</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>41</v>
@@ -1722,7 +1748,7 @@
         <v>15.6</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="P4" s="2">
         <v>41</v>
@@ -1738,12 +1764,12 @@
       </c>
       <c r="Q5" s="3"/>
       <c r="R5" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S5" s="9"/>
       <c r="T5" s="9"/>
     </row>
-    <row r="6" spans="1:20" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" s="21" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>17</v>
       </c>
@@ -1766,7 +1792,7 @@
         <v>20</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>42</v>
+        <v>186</v>
       </c>
       <c r="I6" s="21" t="s">
         <v>41</v>
@@ -1781,23 +1807,33 @@
         <v>31</v>
       </c>
       <c r="M6" s="21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>32</v>
+        <v>184</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="P6" s="21">
+        <v>46</v>
       </c>
       <c r="Q6" s="22">
         <v>0.96</v>
       </c>
       <c r="R6" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
+        <v>65</v>
+      </c>
+      <c r="S6" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="T6" s="49" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="7" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C7" s="2">
         <v>5979</v>
@@ -1815,7 +1851,7 @@
         <v>20</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>41</v>
@@ -1839,7 +1875,7 @@
     </row>
     <row r="8" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="2">
         <v>5379</v>
@@ -1854,10 +1890,10 @@
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>41</v>
@@ -1869,7 +1905,7 @@
         <v>38</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>32</v>
@@ -1883,13 +1919,13 @@
     </row>
     <row r="9" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="2">
         <v>4979</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E9" s="2">
         <v>8</v>
@@ -1898,10 +1934,10 @@
         <v>27</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>41</v>
@@ -1913,167 +1949,121 @@
         <v>38</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>32</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q9" s="3"/>
       <c r="R9" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S9" s="9"/>
       <c r="T9" s="9"/>
     </row>
-    <row r="10" spans="1:20" s="21" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B10" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="21">
-        <v>5999</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E10" s="21">
+    <row r="11" spans="1:20" s="46" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="46" t="s">
+        <v>183</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="46">
+        <v>6779</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="46">
         <v>16</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F11" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="J10" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="K10" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="L10" s="21" t="s">
+      <c r="G11" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="46">
+        <v>25</v>
+      </c>
+      <c r="L11" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="M11" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="N11" s="46">
+        <v>3.4</v>
+      </c>
+      <c r="O11" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="P11" s="46">
+        <v>55</v>
+      </c>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="M10" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="N10" s="21">
-        <v>2</v>
-      </c>
-      <c r="O10" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q10" s="22">
-        <v>43618</v>
-      </c>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="T10" s="23"/>
-    </row>
-    <row r="11" spans="1:20" s="45" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="45" t="s">
-        <v>186</v>
-      </c>
-      <c r="B11" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="45">
-        <v>6779</v>
-      </c>
-      <c r="D11" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="45">
-        <v>16</v>
-      </c>
-      <c r="F11" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="J11" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="K11" s="45">
-        <v>25</v>
-      </c>
-      <c r="L11" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="M11" s="45" t="s">
-        <v>176</v>
-      </c>
-      <c r="N11" s="45">
-        <v>3.4</v>
-      </c>
-      <c r="O11" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="P11" s="45">
-        <v>55</v>
-      </c>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="S11" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="T11" s="47"/>
+      <c r="S11" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="T11" s="48"/>
     </row>
     <row r="12" spans="1:20" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="48" t="s">
-        <v>177</v>
+      <c r="B12" s="45" t="s">
+        <v>191</v>
       </c>
       <c r="C12" s="26">
         <v>5679</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="26">
         <v>8</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G12" s="26" t="s">
         <v>20</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I12" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="K12" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="K12" s="26" t="s">
+      <c r="L12" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="L12" s="26" t="s">
-        <v>77</v>
-      </c>
       <c r="M12" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N12" s="26">
         <v>2.7</v>
+      </c>
+      <c r="O12" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="P12" s="26">
+        <v>62</v>
       </c>
       <c r="Q12" s="27">
         <v>43588</v>
@@ -2083,7 +2073,7 @@
       <c r="T12" s="28"/>
     </row>
     <row r="13" spans="1:20" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="48"/>
+      <c r="B13" s="45"/>
       <c r="Q13" s="27"/>
       <c r="R13" s="28"/>
       <c r="S13" s="28"/>
@@ -2091,25 +2081,25 @@
     </row>
     <row r="14" spans="1:20" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="35" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C14" s="35">
         <v>6799</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E14" s="35">
         <v>16</v>
       </c>
       <c r="F14" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G14" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H14" s="35" t="s">
         <v>24</v>
@@ -2121,19 +2111,19 @@
         <v>29</v>
       </c>
       <c r="K14" s="35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L14" s="35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M14" s="35" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="N14" s="35">
         <v>2</v>
       </c>
       <c r="O14" s="35" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="P14" s="35">
         <v>46</v>
@@ -2141,375 +2131,380 @@
       <c r="Q14" s="36"/>
       <c r="R14" s="37"/>
       <c r="S14" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="T14" s="37"/>
+    </row>
+    <row r="15" spans="1:20" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B15" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="26">
+        <v>6999</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="26">
+        <v>8</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="M15" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+    </row>
+    <row r="16" spans="1:20" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="L16" s="24"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+    </row>
+    <row r="17" spans="1:20" s="29" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="29">
+        <v>5999</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17" s="29">
+        <v>16</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="L17" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="M17" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="N17" s="29">
+        <v>2</v>
+      </c>
+      <c r="O17" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q17" s="30">
+        <v>43618</v>
+      </c>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="T17" s="31"/>
+    </row>
+    <row r="18" spans="1:20" s="32" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="C18" s="32">
+        <v>6199</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="32">
+        <v>8</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="K18" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="L18" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="M18" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="N18" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="O18" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="34"/>
+      <c r="T18" s="34"/>
+    </row>
+    <row r="19" spans="1:20" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="T14" s="37"/>
-    </row>
-    <row r="15" spans="1:20" s="32" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="32" t="s">
+      <c r="B19" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="C19" s="42">
+        <v>6799</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="42">
+        <v>16</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="42" t="s">
+        <v>182</v>
+      </c>
+      <c r="J19" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="L19" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="B15" s="32" t="s">
-        <v>136</v>
-      </c>
-      <c r="C15" s="32">
-        <v>6199</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="32">
+      <c r="N19" s="42">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="44"/>
+      <c r="S19" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="T19" s="44"/>
+    </row>
+    <row r="20" spans="1:20" s="32" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="32">
         <v>8</v>
       </c>
-      <c r="F15" s="32" t="s">
+      <c r="F20" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="J15" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="K15" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="L15" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="M15" s="32" t="s">
+      <c r="G20" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="J20" s="32">
+        <v>17.3</v>
+      </c>
+      <c r="K20" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="M20" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="N20" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="N15" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="O15" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="34"/>
-      <c r="T15" s="34"/>
-    </row>
-    <row r="16" spans="1:20" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="42" t="s">
+      <c r="O20" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="P20" s="32">
+        <v>43</v>
+      </c>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="B16" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="C16" s="42">
-        <v>6799</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="42">
-        <v>16</v>
-      </c>
-      <c r="F16" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="42" t="s">
-        <v>185</v>
-      </c>
-      <c r="J16" s="42" t="s">
-        <v>152</v>
-      </c>
-      <c r="L16" s="42" t="s">
-        <v>147</v>
-      </c>
-      <c r="N16" s="42">
-        <v>4</v>
-      </c>
-      <c r="Q16" s="43"/>
-      <c r="R16" s="44"/>
-      <c r="S16" s="44" t="s">
-        <v>182</v>
-      </c>
-      <c r="T16" s="44"/>
-    </row>
-    <row r="17" spans="1:20" s="32" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="32">
-        <v>8</v>
-      </c>
-      <c r="F17" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="J17" s="32">
-        <v>17.3</v>
-      </c>
-      <c r="K17" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="M17" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="N17" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="O17" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="P17" s="32">
-        <v>43</v>
-      </c>
-      <c r="Q17" s="33"/>
-      <c r="R17" s="34"/>
-      <c r="S17" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="T17" s="34"/>
-    </row>
-    <row r="18" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C18" s="2">
+      <c r="T20" s="34"/>
+    </row>
+    <row r="21" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C21" s="2">
         <v>7699</v>
       </c>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-    </row>
-    <row r="19" spans="1:20" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B19" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="C19" s="26">
-        <v>6999</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="26">
-        <v>8</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="J19" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="L19" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="M19" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="28"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="28"/>
-    </row>
-    <row r="20" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="Q20" s="3"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-    </row>
-    <row r="21" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="Q21" s="3"/>
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
       <c r="T21" s="9"/>
     </row>
-    <row r="22" spans="1:20" s="29" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="38" t="s">
+    <row r="22" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="Q22" s="3"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+    </row>
+    <row r="23" spans="1:20" s="29" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="29">
+        <v>6059</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="29">
+        <v>8</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="29">
-        <v>6059</v>
-      </c>
-      <c r="D22" s="29" t="s">
+      <c r="K23" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="L23" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="M23" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="N23" s="29">
+        <v>1.82</v>
+      </c>
+      <c r="O23" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="29">
+      <c r="P23" s="29">
+        <v>46</v>
+      </c>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="S23" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="T23" s="40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" s="2">
+        <v>7299</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="2">
         <v>8</v>
       </c>
-      <c r="F22" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="I22" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="J22" s="29" t="s">
+      <c r="F24" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K22" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="L22" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="M22" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="N22" s="29">
-        <v>1.82</v>
-      </c>
-      <c r="O22" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="P22" s="29">
-        <v>46</v>
-      </c>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="S22" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="T22" s="40" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B23" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C23" s="2">
-        <v>7299</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="2">
-        <v>8</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="G23" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J23" s="2" t="s">
+      <c r="L24" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="K23" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="T23" s="9"/>
-    </row>
-    <row r="24" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M24" s="2" t="s">
+        <v>168</v>
+      </c>
       <c r="Q24" s="3"/>
       <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
+      <c r="S24" s="9" t="s">
+        <v>180</v>
+      </c>
       <c r="T24" s="9"/>
     </row>
-    <row r="25" spans="1:20" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="Q25" s="3"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+    </row>
+    <row r="26" spans="1:20" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="2">
+        <v>5525</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C25" s="2">
-        <v>5525</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" s="2">
-        <v>8</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="N25" s="2">
-        <v>2.7</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q25" s="3">
-        <v>43588</v>
-      </c>
-      <c r="R25" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="S25" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="T25" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B26" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" s="2">
-        <v>6499</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="E26" s="2">
         <v>8</v>
@@ -2521,27 +2516,48 @@
         <v>21</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="9"/>
+        <v>89</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N26" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>43588</v>
+      </c>
+      <c r="R26" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="S26" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="T26" s="9"/>
+        <v>132</v>
+      </c>
+      <c r="T26" s="5" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="27" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="C27" s="2">
-        <v>5999</v>
+        <v>6499</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E27" s="2">
         <v>8</v>
@@ -2553,31 +2569,57 @@
         <v>21</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>127</v>
+        <v>46</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="N27" s="2">
-        <v>2.35</v>
+        <v>108</v>
       </c>
       <c r="Q27" s="3"/>
       <c r="R27" s="9"/>
       <c r="S27" s="9" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="T27" s="9"/>
     </row>
     <row r="28" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="2">
+        <v>5999</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="2">
+        <v>8</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="N28" s="2">
+        <v>2.35</v>
+      </c>
       <c r="Q28" s="3"/>
       <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
+      <c r="S28" s="9" t="s">
+        <v>127</v>
+      </c>
       <c r="T28" s="9"/>
     </row>
     <row r="29" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2586,149 +2628,146 @@
       <c r="S29" s="9"/>
       <c r="T29" s="9"/>
     </row>
-    <row r="30" spans="1:20" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" s="12" t="s">
+    <row r="30" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="Q30" s="3"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+    </row>
+    <row r="31" spans="1:20" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="C30" s="2">
+      <c r="B31" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="2">
         <v>5999</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F30" s="2" t="s">
+      <c r="D31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="F31" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J30" s="2" t="s">
+      <c r="H31" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="L31" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N31" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O31" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="L30" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="N30" s="2">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="P30" s="2">
+      <c r="P31" s="2">
         <v>52</v>
       </c>
-      <c r="Q30" s="3">
+      <c r="Q31" s="3">
         <v>43588</v>
       </c>
-      <c r="R30" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="S30" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="T30" s="19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="C31" s="2">
+      <c r="R31" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="S31" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="T31" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="14"/>
+      <c r="B32" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="2">
         <v>6099</v>
-      </c>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="19"/>
-    </row>
-    <row r="32" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B32" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" s="2">
-        <v>6699</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J32" s="2">
-        <v>17.3</v>
-      </c>
-      <c r="K32" s="2">
-        <v>25</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="N32" s="2">
-        <v>2.75</v>
       </c>
       <c r="Q32" s="3"/>
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
-      <c r="T32" s="9" t="s">
-        <v>101</v>
-      </c>
+      <c r="T32" s="19"/>
     </row>
     <row r="33" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B33" s="10" t="s">
+        <v>99</v>
+      </c>
       <c r="C33" s="2">
         <v>6699</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E33" s="2">
-        <v>8</v>
+        <v>84</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
+      </c>
+      <c r="J33" s="2">
+        <v>17.3</v>
       </c>
       <c r="K33" s="2">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N33" s="2">
+        <v>2.75</v>
       </c>
       <c r="Q33" s="3"/>
       <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
+      <c r="S33" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="T33" s="9"/>
     </row>
     <row r="34" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B34" s="2" t="s">
-        <v>103</v>
+      <c r="C34" s="2">
+        <v>6699</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="2">
+        <v>8</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K34" s="2">
+        <v>24</v>
       </c>
       <c r="Q34" s="3"/>
       <c r="R34" s="9"/>
@@ -2736,102 +2775,105 @@
       <c r="T34" s="9"/>
     </row>
     <row r="35" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B35" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="Q35" s="3"/>
       <c r="R35" s="9"/>
       <c r="S35" s="9"/>
       <c r="T35" s="9"/>
     </row>
     <row r="36" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C36" s="2">
-        <v>6299</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E36" s="2">
-        <v>8</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="N36" s="2">
-        <v>2.2999999999999998</v>
-      </c>
       <c r="Q36" s="3"/>
       <c r="R36" s="9"/>
-      <c r="S36" s="9" t="s">
-        <v>126</v>
-      </c>
+      <c r="S36" s="9"/>
       <c r="T36" s="9"/>
     </row>
     <row r="37" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" s="2">
+        <v>6299</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E37" s="2">
+        <v>8</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="N37" s="2">
+        <v>2.2999999999999998</v>
+      </c>
       <c r="Q37" s="3"/>
       <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
+      <c r="S37" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="T37" s="9"/>
     </row>
-    <row r="38" spans="1:20" s="29" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="29" t="s">
+    <row r="38" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="Q38" s="3"/>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="9"/>
+    </row>
+    <row r="39" spans="1:20" s="29" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="C39" s="29">
+        <v>6199</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="29">
+        <v>8</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="I39" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="J39" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="C38" s="29">
-        <v>6199</v>
-      </c>
-      <c r="D38" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="E38" s="29">
-        <v>8</v>
-      </c>
-      <c r="F38" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="H38" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="I38" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="J38" s="29" t="s">
+      <c r="O39" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="O38" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q38" s="30"/>
-      <c r="R38" s="31"/>
-      <c r="S38" s="31"/>
-      <c r="T38" s="31"/>
-    </row>
-    <row r="39" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="Q39" s="3"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="9"/>
-      <c r="T39" s="9"/>
+      <c r="Q39" s="30"/>
+      <c r="R39" s="31"/>
+      <c r="S39" s="31"/>
+      <c r="T39" s="31"/>
     </row>
     <row r="40" spans="1:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="Q40" s="3"/>
@@ -3319,14 +3361,21 @@
       <c r="S120" s="9"/>
       <c r="T120" s="9"/>
     </row>
+    <row r="121" spans="17:20" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="Q121" s="3"/>
+      <c r="R121" s="9"/>
+      <c r="S121" s="9"/>
+      <c r="T121" s="9"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="T2" r:id="rId1"/>
-    <hyperlink ref="T22" r:id="rId2"/>
-    <hyperlink ref="T30" r:id="rId3"/>
+    <hyperlink ref="T23" r:id="rId2"/>
+    <hyperlink ref="T31" r:id="rId3"/>
+    <hyperlink ref="T6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>